<commit_message>
Add labor force data
</commit_message>
<xml_diff>
--- a/data/labor_force_state.xlsx
+++ b/data/labor_force_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PSG24/Dropbox/GoogleTrendsUINowcast/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251E159C-63FD-7849-8292-61CFAE875926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E3058E-5DBB-AE49-9183-E2C518470CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{2E104B08-CFB7-1141-90B5-91BFA613D3B1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Alabama</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>New York</t>
-  </si>
-  <si>
-    <t>New York City</t>
   </si>
   <si>
     <t>North Carolina</t>
@@ -567,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925D594F-3FB4-8C4A-BE50-E32F48186BE0}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,10 +578,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -856,7 +853,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>4088923</v>
+        <v>5052626</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -864,7 +861,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>5052626</v>
+        <v>403000</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -872,7 +869,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>403000</v>
+        <v>5798120</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -880,7 +877,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>5798120</v>
+        <v>1837111</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -888,7 +885,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>1837111</v>
+        <v>2107405</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -896,7 +893,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>2107405</v>
+        <v>6452662</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -904,7 +901,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>6452662</v>
+        <v>554644</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -912,7 +909,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>554644</v>
+        <v>2370060</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -920,7 +917,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>2370060</v>
+        <v>461922</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -928,7 +925,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>461922</v>
+        <v>3317224</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -936,7 +933,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>3317224</v>
+        <v>13939304</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -944,7 +941,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>13939304</v>
+        <v>1589639</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -952,7 +949,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>1589639</v>
+        <v>344021</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -960,7 +957,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>344021</v>
+        <v>4381973</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -968,7 +965,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>4381973</v>
+        <v>3875991</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -976,7 +973,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>3875991</v>
+        <v>790807</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -984,7 +981,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>790807</v>
+        <v>3105384</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -992,14 +989,6 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>3105384</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="3">
         <v>291491</v>
       </c>
     </row>

</xml_diff>